<commit_message>
feat: Implement Cache Manager for SQL queries, add configuration and database service
- Added CacheManager class for managing SQL query caching with disk storage.
- Introduced config.py for centralized configuration management including database and cache settings.
- Created DatabaseService class for handling database connections and queries.
- Added list_models.py script to list available models from Google Gemini.
- Developed LLMService class for integrating with Ollama and Google Gemini for SQL generation.
- Updated requirements.txt with necessary dependencies.
- Removed temporary Excel file.
</commit_message>
<xml_diff>
--- a/Relatorio_TLLF_COMPLETO_20251218_115253.xlsx
+++ b/Relatorio_TLLF_COMPLETO_20251218_115253.xlsx
@@ -8,27 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fiscal\PROJETOS\mcp.local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B87D047-8843-4147-86A5-968CAE366F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA52CD2-1CCB-43F5-8CAF-DF003A623314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo Geral" sheetId="1" r:id="rId1"/>
     <sheet name="TLLF 2025 Completo" sheetId="2" r:id="rId2"/>
-    <sheet name="Planilha1" sheetId="6" r:id="rId3"/>
-    <sheet name="TLLF 2024 Completo" sheetId="3" r:id="rId4"/>
-    <sheet name="Em Aberto" sheetId="4" r:id="rId5"/>
-    <sheet name="Análise por Contribuinte" sheetId="5" r:id="rId6"/>
+    <sheet name="TLLF 2024 Completo" sheetId="3" r:id="rId3"/>
+    <sheet name="Em Aberto" sheetId="4" r:id="rId4"/>
+    <sheet name="Análise por Contribuinte" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TLLF 2024 Completo'!$A$3:$J$257</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TLLF 2025 Completo'!$A$1:$J$233</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3989" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3939" uniqueCount="975">
   <si>
     <t>RELATÓRIO COMPLETO TLLF - TODOS OS CONTRIBUINTES</t>
   </si>
@@ -3136,12 +3136,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -3154,6 +3148,12 @@
     <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -3460,7 +3460,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3477,16 +3477,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3662,8 +3662,8 @@
   <dimension ref="A1:J233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A186" sqref="A186:XFD186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3727,7 +3727,7 @@
       <c r="E2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="21">
         <v>1763370</v>
       </c>
       <c r="G2" s="6">
@@ -3759,7 +3759,7 @@
       <c r="E3" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="22">
         <v>1568952</v>
       </c>
       <c r="G3" s="9">
@@ -3791,7 +3791,7 @@
       <c r="E4" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="21">
         <v>1114923.6000000001</v>
       </c>
       <c r="G4" s="6">
@@ -3823,7 +3823,7 @@
       <c r="E5" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="21">
         <v>98789.67</v>
       </c>
       <c r="G5" s="6">
@@ -3855,7 +3855,7 @@
       <c r="E6" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="21">
         <v>97380.89</v>
       </c>
       <c r="G6" s="6">
@@ -3887,7 +3887,7 @@
       <c r="E7" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="21">
         <v>47889.45</v>
       </c>
       <c r="G7" s="6">
@@ -3919,7 +3919,7 @@
       <c r="E8" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="22">
         <v>42288.77</v>
       </c>
       <c r="G8" s="9">
@@ -3951,7 +3951,7 @@
       <c r="E9" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="21">
         <v>12851.37</v>
       </c>
       <c r="G9" s="6">
@@ -3983,7 +3983,7 @@
       <c r="E10" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="21">
         <v>6864.14</v>
       </c>
       <c r="G10" s="6">
@@ -4015,7 +4015,7 @@
       <c r="E11" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="21">
         <v>4725</v>
       </c>
       <c r="G11" s="6">
@@ -4047,7 +4047,7 @@
       <c r="E12" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="21">
         <v>4432.84</v>
       </c>
       <c r="G12" s="6">
@@ -4079,7 +4079,7 @@
       <c r="E13" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="21">
         <v>2945.25</v>
       </c>
       <c r="G13" s="6">
@@ -4111,7 +4111,7 @@
       <c r="E14" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="21">
         <v>2945.25</v>
       </c>
       <c r="G14" s="6">
@@ -4143,7 +4143,7 @@
       <c r="E15" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="21">
         <v>2763.12</v>
       </c>
       <c r="G15" s="6">
@@ -4175,7 +4175,7 @@
       <c r="E16" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="21">
         <v>2701.72</v>
       </c>
       <c r="G16" s="6">
@@ -4207,7 +4207,7 @@
       <c r="E17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="21">
         <v>2701.69</v>
       </c>
       <c r="G17" s="6">
@@ -4239,7 +4239,7 @@
       <c r="E18" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="21">
         <v>2362.5</v>
       </c>
       <c r="G18" s="6">
@@ -4271,7 +4271,7 @@
       <c r="E19" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="21">
         <v>2362.5</v>
       </c>
       <c r="G19" s="6">
@@ -4303,7 +4303,7 @@
       <c r="E20" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="21">
         <v>1957.85</v>
       </c>
       <c r="G20" s="6">
@@ -4335,7 +4335,7 @@
       <c r="E21" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="21">
         <v>1862.78</v>
       </c>
       <c r="G21" s="6">
@@ -4367,7 +4367,7 @@
       <c r="E22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="21">
         <v>1748.25</v>
       </c>
       <c r="G22" s="6">
@@ -4399,7 +4399,7 @@
       <c r="E23" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="21">
         <v>1612.48</v>
       </c>
       <c r="G23" s="6">
@@ -4431,7 +4431,7 @@
       <c r="E24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="21">
         <v>1599.12</v>
       </c>
       <c r="G24" s="6">
@@ -4463,7 +4463,7 @@
       <c r="E25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="21">
         <v>1336.77</v>
       </c>
       <c r="G25" s="6">
@@ -4495,7 +4495,7 @@
       <c r="E26" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="21">
         <v>1335.6</v>
       </c>
       <c r="G26" s="6">
@@ -4527,7 +4527,7 @@
       <c r="E27" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="19">
         <v>1335.6</v>
       </c>
       <c r="G27" s="12">
@@ -4559,7 +4559,7 @@
       <c r="E28" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="19">
         <v>1335.6</v>
       </c>
       <c r="G28" s="12">
@@ -4591,7 +4591,7 @@
       <c r="E29" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="19">
         <v>1335.6</v>
       </c>
       <c r="G29" s="12">
@@ -4623,7 +4623,7 @@
       <c r="E30" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="21">
         <v>1285.2</v>
       </c>
       <c r="G30" s="6">
@@ -4655,7 +4655,7 @@
       <c r="E31" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="21">
         <v>1260</v>
       </c>
       <c r="G31" s="6">
@@ -4687,7 +4687,7 @@
       <c r="E32" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="21">
         <v>1135.26</v>
       </c>
       <c r="G32" s="6">
@@ -4719,7 +4719,7 @@
       <c r="E33" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="21">
         <v>1135.26</v>
       </c>
       <c r="G33" s="6">
@@ -4751,7 +4751,7 @@
       <c r="E34" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="21">
         <v>1135.26</v>
       </c>
       <c r="G34" s="6">
@@ -4783,7 +4783,7 @@
       <c r="E35" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="21">
         <v>1106.79</v>
       </c>
       <c r="G35" s="6">
@@ -4815,7 +4815,7 @@
       <c r="E36" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="19">
         <v>1044.23</v>
       </c>
       <c r="G36" s="12">
@@ -4847,7 +4847,7 @@
       <c r="E37" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F37" s="25">
+      <c r="F37" s="21">
         <v>1023.75</v>
       </c>
       <c r="G37" s="6">
@@ -4879,7 +4879,7 @@
       <c r="E38" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="22">
         <v>1023.75</v>
       </c>
       <c r="G38" s="9">
@@ -4911,7 +4911,7 @@
       <c r="E39" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F39" s="26">
+      <c r="F39" s="22">
         <v>976.3</v>
       </c>
       <c r="G39" s="9">
@@ -4943,7 +4943,7 @@
       <c r="E40" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F40" s="25">
+      <c r="F40" s="21">
         <v>968.79</v>
       </c>
       <c r="G40" s="6">
@@ -4975,7 +4975,7 @@
       <c r="E41" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F41" s="25">
+      <c r="F41" s="21">
         <v>952.88</v>
       </c>
       <c r="G41" s="6">
@@ -5007,7 +5007,7 @@
       <c r="E42" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F42" s="25">
+      <c r="F42" s="21">
         <v>944.15</v>
       </c>
       <c r="G42" s="6">
@@ -5039,7 +5039,7 @@
       <c r="E43" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="F43" s="25">
+      <c r="F43" s="21">
         <v>927.49</v>
       </c>
       <c r="G43" s="6">
@@ -5071,7 +5071,7 @@
       <c r="E44" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F44" s="25">
+      <c r="F44" s="21">
         <v>882</v>
       </c>
       <c r="G44" s="6">
@@ -5103,7 +5103,7 @@
       <c r="E45" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="F45" s="25">
+      <c r="F45" s="21">
         <v>803.25</v>
       </c>
       <c r="G45" s="6">
@@ -5135,7 +5135,7 @@
       <c r="E46" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F46" s="25">
+      <c r="F46" s="21">
         <v>787.5</v>
       </c>
       <c r="G46" s="6">
@@ -5167,7 +5167,7 @@
       <c r="E47" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F47" s="25">
+      <c r="F47" s="21">
         <v>787.5</v>
       </c>
       <c r="G47" s="6">
@@ -5199,7 +5199,7 @@
       <c r="E48" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F48" s="25">
+      <c r="F48" s="21">
         <v>787.5</v>
       </c>
       <c r="G48" s="6">
@@ -5231,7 +5231,7 @@
       <c r="E49" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F49" s="25">
+      <c r="F49" s="21">
         <v>787.5</v>
       </c>
       <c r="G49" s="6">
@@ -5263,7 +5263,7 @@
       <c r="E50" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F50" s="25">
+      <c r="F50" s="21">
         <v>787.5</v>
       </c>
       <c r="G50" s="6">
@@ -5295,7 +5295,7 @@
       <c r="E51" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F51" s="25">
+      <c r="F51" s="21">
         <v>787.5</v>
       </c>
       <c r="G51" s="6">
@@ -5327,7 +5327,7 @@
       <c r="E52" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="F52" s="26">
+      <c r="F52" s="22">
         <v>787.5</v>
       </c>
       <c r="G52" s="9">
@@ -5359,7 +5359,7 @@
       <c r="E53" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F53" s="25">
+      <c r="F53" s="21">
         <v>787.5</v>
       </c>
       <c r="G53" s="6">
@@ -5391,7 +5391,7 @@
       <c r="E54" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F54" s="25">
+      <c r="F54" s="21">
         <v>787.5</v>
       </c>
       <c r="G54" s="6">
@@ -5423,7 +5423,7 @@
       <c r="E55" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F55" s="25">
+      <c r="F55" s="21">
         <v>787.5</v>
       </c>
       <c r="G55" s="6">
@@ -5455,7 +5455,7 @@
       <c r="E56" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F56" s="25">
+      <c r="F56" s="21">
         <v>787.5</v>
       </c>
       <c r="G56" s="6">
@@ -5487,7 +5487,7 @@
       <c r="E57" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F57" s="25">
+      <c r="F57" s="21">
         <v>754.42</v>
       </c>
       <c r="G57" s="6">
@@ -5519,7 +5519,7 @@
       <c r="E58" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F58" s="25">
+      <c r="F58" s="21">
         <v>751</v>
       </c>
       <c r="G58" s="6">
@@ -5551,7 +5551,7 @@
       <c r="E59" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F59" s="25">
+      <c r="F59" s="21">
         <v>718</v>
       </c>
       <c r="G59" s="6">
@@ -5583,7 +5583,7 @@
       <c r="E60" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F60" s="25">
+      <c r="F60" s="21">
         <v>715.84</v>
       </c>
       <c r="G60" s="6">
@@ -5615,7 +5615,7 @@
       <c r="E61" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F61" s="25">
+      <c r="F61" s="21">
         <v>708.75</v>
       </c>
       <c r="G61" s="6">
@@ -5647,7 +5647,7 @@
       <c r="E62" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F62" s="24">
+      <c r="F62" s="20">
         <v>614.25</v>
       </c>
       <c r="G62" s="15">
@@ -5679,7 +5679,7 @@
       <c r="E63" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="F63" s="24">
+      <c r="F63" s="20">
         <v>393.75</v>
       </c>
       <c r="G63" s="15">
@@ -5711,7 +5711,7 @@
       <c r="E64" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F64" s="25">
+      <c r="F64" s="21">
         <v>708.75</v>
       </c>
       <c r="G64" s="6">
@@ -5743,7 +5743,7 @@
       <c r="E65" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F65" s="25">
+      <c r="F65" s="21">
         <v>707.82</v>
       </c>
       <c r="G65" s="6">
@@ -5775,7 +5775,7 @@
       <c r="E66" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F66" s="25">
+      <c r="F66" s="21">
         <v>702.13</v>
       </c>
       <c r="G66" s="6">
@@ -5807,7 +5807,7 @@
       <c r="E67" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F67" s="25">
+      <c r="F67" s="21">
         <v>681.77</v>
       </c>
       <c r="G67" s="6">
@@ -5839,7 +5839,7 @@
       <c r="E68" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F68" s="25">
+      <c r="F68" s="21">
         <v>679.39</v>
       </c>
       <c r="G68" s="6">
@@ -5871,7 +5871,7 @@
       <c r="E69" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F69" s="24">
+      <c r="F69" s="20">
         <v>1260</v>
       </c>
       <c r="G69" s="15">
@@ -5903,7 +5903,7 @@
       <c r="E70" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="F70" s="24">
+      <c r="F70" s="20">
         <v>4725</v>
       </c>
       <c r="G70" s="15">
@@ -5935,7 +5935,7 @@
       <c r="E71" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F71" s="25">
+      <c r="F71" s="21">
         <v>665.91</v>
       </c>
       <c r="G71" s="6">
@@ -5967,7 +5967,7 @@
       <c r="E72" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="F72" s="25">
+      <c r="F72" s="21">
         <v>661.5</v>
       </c>
       <c r="G72" s="6">
@@ -5999,7 +5999,7 @@
       <c r="E73" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F73" s="24">
+      <c r="F73" s="20">
         <v>393.75</v>
       </c>
       <c r="G73" s="15">
@@ -6031,7 +6031,7 @@
       <c r="E74" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F74" s="25">
+      <c r="F74" s="21">
         <v>630</v>
       </c>
       <c r="G74" s="6">
@@ -6063,7 +6063,7 @@
       <c r="E75" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="F75" s="24">
+      <c r="F75" s="20">
         <v>4359.6000000000004</v>
       </c>
       <c r="G75" s="15">
@@ -6095,7 +6095,7 @@
       <c r="E76" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="F76" s="25">
+      <c r="F76" s="21">
         <v>630</v>
       </c>
       <c r="G76" s="6">
@@ -6127,7 +6127,7 @@
       <c r="E77" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="F77" s="25">
+      <c r="F77" s="21">
         <v>630</v>
       </c>
       <c r="G77" s="6">
@@ -6159,7 +6159,7 @@
       <c r="E78" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="F78" s="25">
+      <c r="F78" s="21">
         <v>630</v>
       </c>
       <c r="G78" s="6">
@@ -6191,7 +6191,7 @@
       <c r="E79" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F79" s="24">
+      <c r="F79" s="20">
         <v>393.75</v>
       </c>
       <c r="G79" s="15">
@@ -6223,7 +6223,7 @@
       <c r="E80" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F80" s="25">
+      <c r="F80" s="21">
         <v>615.96</v>
       </c>
       <c r="G80" s="6">
@@ -6255,7 +6255,7 @@
       <c r="E81" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F81" s="23">
+      <c r="F81" s="19">
         <v>615.96</v>
       </c>
       <c r="G81" s="12">
@@ -6287,7 +6287,7 @@
       <c r="E82" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F82" s="23">
+      <c r="F82" s="19">
         <v>615.96</v>
       </c>
       <c r="G82" s="12">
@@ -6319,7 +6319,7 @@
       <c r="E83" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F83" s="24">
+      <c r="F83" s="20">
         <v>393.75</v>
       </c>
       <c r="G83" s="15">
@@ -6351,7 +6351,7 @@
       <c r="E84" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F84" s="24">
+      <c r="F84" s="20">
         <v>393.75</v>
       </c>
       <c r="G84" s="15">
@@ -6383,7 +6383,7 @@
       <c r="E85" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F85" s="24">
+      <c r="F85" s="20">
         <v>393.75</v>
       </c>
       <c r="G85" s="15">
@@ -6415,7 +6415,7 @@
       <c r="E86" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F86" s="23">
+      <c r="F86" s="19">
         <v>615.96</v>
       </c>
       <c r="G86" s="12">
@@ -6447,7 +6447,7 @@
       <c r="E87" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F87" s="23">
+      <c r="F87" s="19">
         <v>615.96</v>
       </c>
       <c r="G87" s="12">
@@ -6479,7 +6479,7 @@
       <c r="E88" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F88" s="26">
+      <c r="F88" s="22">
         <v>600.08000000000004</v>
       </c>
       <c r="G88" s="9">
@@ -6511,7 +6511,7 @@
       <c r="E89" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F89" s="26">
+      <c r="F89" s="22">
         <v>600.08000000000004</v>
       </c>
       <c r="G89" s="9">
@@ -6543,7 +6543,7 @@
       <c r="E90" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="F90" s="23">
+      <c r="F90" s="19">
         <v>600.08000000000004</v>
       </c>
       <c r="G90" s="12">
@@ -6575,7 +6575,7 @@
       <c r="E91" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="F91" s="23">
+      <c r="F91" s="19">
         <v>600.08000000000004</v>
       </c>
       <c r="G91" s="12">
@@ -6607,7 +6607,7 @@
       <c r="E92" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F92" s="25">
+      <c r="F92" s="21">
         <v>597.48</v>
       </c>
       <c r="G92" s="6">
@@ -6639,7 +6639,7 @@
       <c r="E93" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F93" s="25">
+      <c r="F93" s="21">
         <v>520.70000000000005</v>
       </c>
       <c r="G93" s="6">
@@ -6671,7 +6671,7 @@
       <c r="E94" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F94" s="25">
+      <c r="F94" s="21">
         <v>518.16999999999996</v>
       </c>
       <c r="G94" s="6">
@@ -6703,7 +6703,7 @@
       <c r="E95" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F95" s="25">
+      <c r="F95" s="21">
         <v>516.6</v>
       </c>
       <c r="G95" s="6">
@@ -6735,7 +6735,7 @@
       <c r="E96" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="F96" s="25">
+      <c r="F96" s="21">
         <v>516.05999999999995</v>
       </c>
       <c r="G96" s="6">
@@ -6767,7 +6767,7 @@
       <c r="E97" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="F97" s="25">
+      <c r="F97" s="21">
         <v>481.55</v>
       </c>
       <c r="G97" s="6">
@@ -6799,7 +6799,7 @@
       <c r="E98" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F98" s="25">
+      <c r="F98" s="21">
         <v>471.62</v>
       </c>
       <c r="G98" s="6">
@@ -6831,7 +6831,7 @@
       <c r="E99" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F99" s="25">
+      <c r="F99" s="21">
         <v>463.52</v>
       </c>
       <c r="G99" s="6">
@@ -6863,7 +6863,7 @@
       <c r="E100" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="F100" s="25">
+      <c r="F100" s="21">
         <v>456.75</v>
       </c>
       <c r="G100" s="6">
@@ -6895,7 +6895,7 @@
       <c r="E101" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F101" s="25">
+      <c r="F101" s="21">
         <v>452.02</v>
       </c>
       <c r="G101" s="6">
@@ -6927,7 +6927,7 @@
       <c r="E102" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F102" s="25">
+      <c r="F102" s="21">
         <v>451.47</v>
       </c>
       <c r="G102" s="6">
@@ -6959,7 +6959,7 @@
       <c r="E103" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F103" s="25">
+      <c r="F103" s="21">
         <v>449.19</v>
       </c>
       <c r="G103" s="6">
@@ -6991,7 +6991,7 @@
       <c r="E104" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="F104" s="25">
+      <c r="F104" s="21">
         <v>429.98</v>
       </c>
       <c r="G104" s="6">
@@ -7023,7 +7023,7 @@
       <c r="E105" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="F105" s="25">
+      <c r="F105" s="21">
         <v>417.38</v>
       </c>
       <c r="G105" s="6">
@@ -7055,7 +7055,7 @@
       <c r="E106" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F106" s="24">
+      <c r="F106" s="20">
         <v>600.08000000000004</v>
       </c>
       <c r="G106" s="15">
@@ -7087,7 +7087,7 @@
       <c r="E107" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="F107" s="25">
+      <c r="F107" s="21">
         <v>417.38</v>
       </c>
       <c r="G107" s="6">
@@ -7119,7 +7119,7 @@
       <c r="E108" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F108" s="25">
+      <c r="F108" s="21">
         <v>417.38</v>
       </c>
       <c r="G108" s="6">
@@ -7151,7 +7151,7 @@
       <c r="E109" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="F109" s="25">
+      <c r="F109" s="21">
         <v>414.43</v>
       </c>
       <c r="G109" s="6">
@@ -7183,7 +7183,7 @@
       <c r="E110" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F110" s="25">
+      <c r="F110" s="21">
         <v>413.44</v>
       </c>
       <c r="G110" s="6">
@@ -7215,7 +7215,7 @@
       <c r="E111" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="F111" s="24">
+      <c r="F111" s="20">
         <v>600.08000000000004</v>
       </c>
       <c r="G111" s="15">
@@ -7247,7 +7247,7 @@
       <c r="E112" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F112" s="25">
+      <c r="F112" s="21">
         <v>393.75</v>
       </c>
       <c r="G112" s="6">
@@ -7279,7 +7279,7 @@
       <c r="E113" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F113" s="25">
+      <c r="F113" s="21">
         <v>393.75</v>
       </c>
       <c r="G113" s="6">
@@ -7311,7 +7311,7 @@
       <c r="E114" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F114" s="25">
+      <c r="F114" s="21">
         <v>393.75</v>
       </c>
       <c r="G114" s="6">
@@ -7343,7 +7343,7 @@
       <c r="E115" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F115" s="25">
+      <c r="F115" s="21">
         <v>393.75</v>
       </c>
       <c r="G115" s="6">
@@ -7375,7 +7375,7 @@
       <c r="E116" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F116" s="25">
+      <c r="F116" s="21">
         <v>393.75</v>
       </c>
       <c r="G116" s="6">
@@ -7407,7 +7407,7 @@
       <c r="E117" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F117" s="25">
+      <c r="F117" s="21">
         <v>393.75</v>
       </c>
       <c r="G117" s="6">
@@ -7439,7 +7439,7 @@
       <c r="E118" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F118" s="25">
+      <c r="F118" s="21">
         <v>393.75</v>
       </c>
       <c r="G118" s="6">
@@ -7471,7 +7471,7 @@
       <c r="E119" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F119" s="25">
+      <c r="F119" s="21">
         <v>393.75</v>
       </c>
       <c r="G119" s="6">
@@ -7503,7 +7503,7 @@
       <c r="E120" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="F120" s="25">
+      <c r="F120" s="21">
         <v>393.75</v>
       </c>
       <c r="G120" s="6">
@@ -7535,7 +7535,7 @@
       <c r="E121" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="F121" s="25">
+      <c r="F121" s="21">
         <v>393.75</v>
       </c>
       <c r="G121" s="6">
@@ -7567,7 +7567,7 @@
       <c r="E122" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F122" s="25">
+      <c r="F122" s="21">
         <v>393.75</v>
       </c>
       <c r="G122" s="6">
@@ -7599,7 +7599,7 @@
       <c r="E123" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="F123" s="25">
+      <c r="F123" s="21">
         <v>393.75</v>
       </c>
       <c r="G123" s="6">
@@ -7631,7 +7631,7 @@
       <c r="E124" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="F124" s="25">
+      <c r="F124" s="21">
         <v>393.75</v>
       </c>
       <c r="G124" s="6">
@@ -7663,7 +7663,7 @@
       <c r="E125" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F125" s="24">
+      <c r="F125" s="20">
         <v>393.75</v>
       </c>
       <c r="G125" s="15">
@@ -7695,7 +7695,7 @@
       <c r="E126" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F126" s="24">
+      <c r="F126" s="20">
         <v>393.75</v>
       </c>
       <c r="G126" s="15">
@@ -7727,7 +7727,7 @@
       <c r="E127" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F127" s="24">
+      <c r="F127" s="20">
         <v>393.75</v>
       </c>
       <c r="G127" s="15">
@@ -7759,7 +7759,7 @@
       <c r="E128" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F128" s="24">
+      <c r="F128" s="20">
         <v>393.75</v>
       </c>
       <c r="G128" s="15">
@@ -7791,7 +7791,7 @@
       <c r="E129" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F129" s="25">
+      <c r="F129" s="21">
         <v>393.75</v>
       </c>
       <c r="G129" s="6">
@@ -7823,7 +7823,7 @@
       <c r="E130" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F130" s="25">
+      <c r="F130" s="21">
         <v>393.75</v>
       </c>
       <c r="G130" s="6">
@@ -7855,7 +7855,7 @@
       <c r="E131" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F131" s="25">
+      <c r="F131" s="21">
         <v>393.75</v>
       </c>
       <c r="G131" s="6">
@@ -7887,7 +7887,7 @@
       <c r="E132" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F132" s="26">
+      <c r="F132" s="22">
         <v>393.75</v>
       </c>
       <c r="G132" s="9">
@@ -7919,7 +7919,7 @@
       <c r="E133" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F133" s="26">
+      <c r="F133" s="22">
         <v>393.75</v>
       </c>
       <c r="G133" s="9">
@@ -7951,7 +7951,7 @@
       <c r="E134" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F134" s="26">
+      <c r="F134" s="22">
         <v>393.75</v>
       </c>
       <c r="G134" s="9">
@@ -7983,7 +7983,7 @@
       <c r="E135" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F135" s="25">
+      <c r="F135" s="21">
         <v>393.75</v>
       </c>
       <c r="G135" s="6">
@@ -8015,7 +8015,7 @@
       <c r="E136" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="F136" s="23">
+      <c r="F136" s="19">
         <v>393.75</v>
       </c>
       <c r="G136" s="12">
@@ -8047,7 +8047,7 @@
       <c r="E137" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="F137" s="23">
+      <c r="F137" s="19">
         <v>393.75</v>
       </c>
       <c r="G137" s="12">
@@ -8079,7 +8079,7 @@
       <c r="E138" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="F138" s="25">
+      <c r="F138" s="21">
         <v>393.75</v>
       </c>
       <c r="G138" s="6">
@@ -8111,7 +8111,7 @@
       <c r="E139" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F139" s="25">
+      <c r="F139" s="21">
         <v>393.75</v>
       </c>
       <c r="G139" s="6">
@@ -8143,7 +8143,7 @@
       <c r="E140" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F140" s="25">
+      <c r="F140" s="21">
         <v>393.75</v>
       </c>
       <c r="G140" s="6">
@@ -8175,7 +8175,7 @@
       <c r="E141" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F141" s="25">
+      <c r="F141" s="21">
         <v>393.75</v>
       </c>
       <c r="G141" s="6">
@@ -8207,7 +8207,7 @@
       <c r="E142" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="F142" s="25">
+      <c r="F142" s="21">
         <v>393.75</v>
       </c>
       <c r="G142" s="6">
@@ -8239,7 +8239,7 @@
       <c r="E143" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="F143" s="25">
+      <c r="F143" s="21">
         <v>393.75</v>
       </c>
       <c r="G143" s="6">
@@ -8271,7 +8271,7 @@
       <c r="E144" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F144" s="25">
+      <c r="F144" s="21">
         <v>393.75</v>
       </c>
       <c r="G144" s="6">
@@ -8303,7 +8303,7 @@
       <c r="E145" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F145" s="25">
+      <c r="F145" s="21">
         <v>393.75</v>
       </c>
       <c r="G145" s="6">
@@ -8335,7 +8335,7 @@
       <c r="E146" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="F146" s="25">
+      <c r="F146" s="21">
         <v>393.75</v>
       </c>
       <c r="G146" s="6">
@@ -8367,7 +8367,7 @@
       <c r="E147" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F147" s="25">
+      <c r="F147" s="21">
         <v>393.75</v>
       </c>
       <c r="G147" s="6">
@@ -8399,7 +8399,7 @@
       <c r="E148" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="F148" s="26">
+      <c r="F148" s="22">
         <v>393.75</v>
       </c>
       <c r="G148" s="9">
@@ -8431,7 +8431,7 @@
       <c r="E149" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="F149" s="24">
+      <c r="F149" s="20">
         <v>740.25</v>
       </c>
       <c r="G149" s="15">
@@ -8463,7 +8463,7 @@
       <c r="E150" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F150" s="26">
+      <c r="F150" s="22">
         <v>393.75</v>
       </c>
       <c r="G150" s="9">
@@ -8495,7 +8495,7 @@
       <c r="E151" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F151" s="25">
+      <c r="F151" s="21">
         <v>393.75</v>
       </c>
       <c r="G151" s="6">
@@ -8527,7 +8527,7 @@
       <c r="E152" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F152" s="25">
+      <c r="F152" s="21">
         <v>393.75</v>
       </c>
       <c r="G152" s="6">
@@ -8559,7 +8559,7 @@
       <c r="E153" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F153" s="25">
+      <c r="F153" s="21">
         <v>393.75</v>
       </c>
       <c r="G153" s="6">
@@ -8591,7 +8591,7 @@
       <c r="E154" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="F154" s="25">
+      <c r="F154" s="21">
         <v>393.75</v>
       </c>
       <c r="G154" s="6">
@@ -8623,7 +8623,7 @@
       <c r="E155" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="F155" s="24">
+      <c r="F155" s="20">
         <v>315</v>
       </c>
       <c r="G155" s="15">
@@ -8655,7 +8655,7 @@
       <c r="E156" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F156" s="25">
+      <c r="F156" s="21">
         <v>393.75</v>
       </c>
       <c r="G156" s="6">
@@ -8687,7 +8687,7 @@
       <c r="E157" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F157" s="25">
+      <c r="F157" s="21">
         <v>393.75</v>
       </c>
       <c r="G157" s="6">
@@ -8719,7 +8719,7 @@
       <c r="E158" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F158" s="25">
+      <c r="F158" s="21">
         <v>393.75</v>
       </c>
       <c r="G158" s="6">
@@ -8751,7 +8751,7 @@
       <c r="E159" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="F159" s="25">
+      <c r="F159" s="21">
         <v>393.75</v>
       </c>
       <c r="G159" s="6">
@@ -8783,7 +8783,7 @@
       <c r="E160" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F160" s="25">
+      <c r="F160" s="21">
         <v>393.75</v>
       </c>
       <c r="G160" s="6">
@@ -8815,7 +8815,7 @@
       <c r="E161" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F161" s="25">
+      <c r="F161" s="21">
         <v>393.75</v>
       </c>
       <c r="G161" s="6">
@@ -8847,7 +8847,7 @@
       <c r="E162" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F162" s="25">
+      <c r="F162" s="21">
         <v>393.75</v>
       </c>
       <c r="G162" s="6">
@@ -8879,7 +8879,7 @@
       <c r="E163" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F163" s="25">
+      <c r="F163" s="21">
         <v>393.75</v>
       </c>
       <c r="G163" s="6">
@@ -8911,7 +8911,7 @@
       <c r="E164" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="F164" s="25">
+      <c r="F164" s="21">
         <v>393.75</v>
       </c>
       <c r="G164" s="6">
@@ -8943,7 +8943,7 @@
       <c r="E165" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F165" s="25">
+      <c r="F165" s="21">
         <v>393.75</v>
       </c>
       <c r="G165" s="6">
@@ -8975,7 +8975,7 @@
       <c r="E166" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="F166" s="25">
+      <c r="F166" s="21">
         <v>389.18</v>
       </c>
       <c r="G166" s="6">
@@ -9007,7 +9007,7 @@
       <c r="E167" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="F167" s="25">
+      <c r="F167" s="21">
         <v>384.3</v>
       </c>
       <c r="G167" s="6">
@@ -9039,7 +9039,7 @@
       <c r="E168" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F168" s="25">
+      <c r="F168" s="21">
         <v>375.5</v>
       </c>
       <c r="G168" s="6">
@@ -9071,7 +9071,7 @@
       <c r="E169" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F169" s="25">
+      <c r="F169" s="21">
         <v>375.5</v>
       </c>
       <c r="G169" s="6">
@@ -9103,7 +9103,7 @@
       <c r="E170" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="F170" s="25">
+      <c r="F170" s="21">
         <v>375.5</v>
       </c>
       <c r="G170" s="6">
@@ -9135,7 +9135,7 @@
       <c r="E171" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F171" s="25">
+      <c r="F171" s="21">
         <v>375.5</v>
       </c>
       <c r="G171" s="6">
@@ -9167,7 +9167,7 @@
       <c r="E172" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F172" s="25">
+      <c r="F172" s="21">
         <v>375.05</v>
       </c>
       <c r="G172" s="6">
@@ -9199,7 +9199,7 @@
       <c r="E173" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F173" s="25">
+      <c r="F173" s="21">
         <v>351.74</v>
       </c>
       <c r="G173" s="6">
@@ -9231,7 +9231,7 @@
       <c r="E174" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F174" s="25">
+      <c r="F174" s="21">
         <v>315</v>
       </c>
       <c r="G174" s="6">
@@ -9263,7 +9263,7 @@
       <c r="E175" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F175" s="26">
+      <c r="F175" s="22">
         <v>315</v>
       </c>
       <c r="G175" s="9">
@@ -9295,7 +9295,7 @@
       <c r="E176" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="F176" s="24">
+      <c r="F176" s="20">
         <v>393.75</v>
       </c>
       <c r="G176" s="15">
@@ -9327,7 +9327,7 @@
       <c r="E177" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F177" s="25">
+      <c r="F177" s="21">
         <v>315</v>
       </c>
       <c r="G177" s="6">
@@ -9359,7 +9359,7 @@
       <c r="E178" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F178" s="25">
+      <c r="F178" s="21">
         <v>315</v>
       </c>
       <c r="G178" s="6">
@@ -9391,7 +9391,7 @@
       <c r="E179" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F179" s="25">
+      <c r="F179" s="21">
         <v>315</v>
       </c>
       <c r="G179" s="6">
@@ -9423,7 +9423,7 @@
       <c r="E180" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F180" s="25">
+      <c r="F180" s="21">
         <v>315</v>
       </c>
       <c r="G180" s="6">
@@ -9455,7 +9455,7 @@
       <c r="E181" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F181" s="25">
+      <c r="F181" s="21">
         <v>315</v>
       </c>
       <c r="G181" s="6">
@@ -9487,7 +9487,7 @@
       <c r="E182" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="F182" s="25">
+      <c r="F182" s="21">
         <v>315</v>
       </c>
       <c r="G182" s="6">
@@ -9519,7 +9519,7 @@
       <c r="E183" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F183" s="25">
+      <c r="F183" s="21">
         <v>315</v>
       </c>
       <c r="G183" s="6">
@@ -9551,7 +9551,7 @@
       <c r="E184" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F184" s="25">
+      <c r="F184" s="21">
         <v>315</v>
       </c>
       <c r="G184" s="6">
@@ -9583,7 +9583,7 @@
       <c r="E185" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F185" s="25">
+      <c r="F185" s="21">
         <v>315</v>
       </c>
       <c r="G185" s="6">
@@ -9615,7 +9615,7 @@
       <c r="E186" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="F186" s="25">
+      <c r="F186" s="21">
         <v>315</v>
       </c>
       <c r="G186" s="6">
@@ -9647,7 +9647,7 @@
       <c r="E187" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="F187" s="23">
+      <c r="F187" s="19">
         <v>315</v>
       </c>
       <c r="G187" s="12">
@@ -9679,7 +9679,7 @@
       <c r="E188" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="F188" s="23">
+      <c r="F188" s="19">
         <v>315</v>
       </c>
       <c r="G188" s="12">
@@ -9711,7 +9711,7 @@
       <c r="E189" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="F189" s="23">
+      <c r="F189" s="19">
         <v>315</v>
       </c>
       <c r="G189" s="12">
@@ -9743,7 +9743,7 @@
       <c r="E190" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="F190" s="24">
+      <c r="F190" s="20">
         <v>315</v>
       </c>
       <c r="G190" s="15">
@@ -9775,7 +9775,7 @@
       <c r="E191" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="F191" s="24">
+      <c r="F191" s="20">
         <v>315</v>
       </c>
       <c r="G191" s="15">
@@ -9807,7 +9807,7 @@
       <c r="E192" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="F192" s="23">
+      <c r="F192" s="19">
         <v>315</v>
       </c>
       <c r="G192" s="12">
@@ -9839,7 +9839,7 @@
       <c r="E193" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F193" s="25">
+      <c r="F193" s="21">
         <v>315</v>
       </c>
       <c r="G193" s="6">
@@ -9871,7 +9871,7 @@
       <c r="E194" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F194" s="25">
+      <c r="F194" s="21">
         <v>315</v>
       </c>
       <c r="G194" s="6">
@@ -9903,7 +9903,7 @@
       <c r="E195" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F195" s="25">
+      <c r="F195" s="21">
         <v>315</v>
       </c>
       <c r="G195" s="6">
@@ -9935,7 +9935,7 @@
       <c r="E196" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="F196" s="26">
+      <c r="F196" s="22">
         <v>315</v>
       </c>
       <c r="G196" s="9">
@@ -9967,7 +9967,7 @@
       <c r="E197" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="F197" s="25">
+      <c r="F197" s="21">
         <v>315</v>
       </c>
       <c r="G197" s="6">
@@ -9999,7 +9999,7 @@
       <c r="E198" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F198" s="25">
+      <c r="F198" s="21">
         <v>300.39999999999998</v>
       </c>
       <c r="G198" s="6">
@@ -10031,7 +10031,7 @@
       <c r="E199" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="F199" s="25">
+      <c r="F199" s="21">
         <v>157.19999999999999</v>
       </c>
       <c r="G199" s="6">
@@ -10063,7 +10063,7 @@
       <c r="E200" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F200" s="25">
+      <c r="F200" s="21">
         <v>31.5</v>
       </c>
       <c r="G200" s="6">
@@ -10095,7 +10095,7 @@
       <c r="E201" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F201" s="25">
+      <c r="F201" s="21">
         <v>31.5</v>
       </c>
       <c r="G201" s="6">
@@ -10127,7 +10127,7 @@
       <c r="E202" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F202" s="25">
+      <c r="F202" s="21">
         <v>31.5</v>
       </c>
       <c r="G202" s="6">
@@ -10159,7 +10159,7 @@
       <c r="E203" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F203" s="25">
+      <c r="F203" s="21">
         <v>31.5</v>
       </c>
       <c r="G203" s="6">
@@ -10191,7 +10191,7 @@
       <c r="E204" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F204" s="25">
+      <c r="F204" s="21">
         <v>31.5</v>
       </c>
       <c r="G204" s="6">
@@ -10223,7 +10223,7 @@
       <c r="E205" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="F205" s="25">
+      <c r="F205" s="21">
         <v>31.5</v>
       </c>
       <c r="G205" s="6">
@@ -10255,7 +10255,7 @@
       <c r="E206" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="F206" s="24">
+      <c r="F206" s="20">
         <v>393.75</v>
       </c>
       <c r="G206" s="15">
@@ -10287,7 +10287,7 @@
       <c r="E207" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="F207" s="24">
+      <c r="F207" s="20">
         <v>393.75</v>
       </c>
       <c r="G207" s="15">
@@ -10319,7 +10319,7 @@
       <c r="E208" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="F208" s="24">
+      <c r="F208" s="20">
         <v>393.75</v>
       </c>
       <c r="G208" s="15">
@@ -10351,7 +10351,7 @@
       <c r="E209" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F209" s="25">
+      <c r="F209" s="21">
         <v>31.5</v>
       </c>
       <c r="G209" s="6">
@@ -10383,7 +10383,7 @@
       <c r="E210" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="F210" s="24">
+      <c r="F210" s="20">
         <v>4725</v>
       </c>
       <c r="G210" s="15">
@@ -10415,7 +10415,7 @@
       <c r="E211" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F211" s="25">
+      <c r="F211" s="21">
         <v>31.5</v>
       </c>
       <c r="G211" s="6">
@@ -10447,7 +10447,7 @@
       <c r="E212" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F212" s="25">
+      <c r="F212" s="21">
         <v>31.5</v>
       </c>
       <c r="G212" s="6">
@@ -10479,7 +10479,7 @@
       <c r="E213" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="F213" s="25">
+      <c r="F213" s="21">
         <v>31.5</v>
       </c>
       <c r="G213" s="6">
@@ -10511,7 +10511,7 @@
       <c r="E214" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F214" s="25">
+      <c r="F214" s="21">
         <v>31.5</v>
       </c>
       <c r="G214" s="6">
@@ -10543,7 +10543,7 @@
       <c r="E215" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F215" s="25">
+      <c r="F215" s="21">
         <v>31.5</v>
       </c>
       <c r="G215" s="6">
@@ -10575,7 +10575,7 @@
       <c r="E216" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F216" s="25">
+      <c r="F216" s="21">
         <v>31.5</v>
       </c>
       <c r="G216" s="6">
@@ -10607,7 +10607,7 @@
       <c r="E217" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="F217" s="24">
+      <c r="F217" s="20">
         <v>1260</v>
       </c>
       <c r="G217" s="15">
@@ -10639,7 +10639,7 @@
       <c r="E218" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F218" s="25">
+      <c r="F218" s="21">
         <v>31.5</v>
       </c>
       <c r="G218" s="6">
@@ -10671,7 +10671,7 @@
       <c r="E219" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F219" s="25">
+      <c r="F219" s="21">
         <v>31.5</v>
       </c>
       <c r="G219" s="6">
@@ -10703,7 +10703,7 @@
       <c r="E220" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F220" s="25">
+      <c r="F220" s="21">
         <v>31.5</v>
       </c>
       <c r="G220" s="6">
@@ -10735,7 +10735,7 @@
       <c r="E221" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="F221" s="25">
+      <c r="F221" s="21">
         <v>31.5</v>
       </c>
       <c r="G221" s="6">
@@ -10767,7 +10767,7 @@
       <c r="E222" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F222" s="25">
+      <c r="F222" s="21">
         <v>31.5</v>
       </c>
       <c r="G222" s="6">
@@ -10799,7 +10799,7 @@
       <c r="E223" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F223" s="25">
+      <c r="F223" s="21">
         <v>31.5</v>
       </c>
       <c r="G223" s="6">
@@ -10831,7 +10831,7 @@
       <c r="E224" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="F224" s="25">
+      <c r="F224" s="21">
         <v>31.5</v>
       </c>
       <c r="G224" s="6">
@@ -10863,7 +10863,7 @@
       <c r="E225" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F225" s="25">
+      <c r="F225" s="21">
         <v>31.5</v>
       </c>
       <c r="G225" s="6">
@@ -10895,7 +10895,7 @@
       <c r="E226" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F226" s="25">
+      <c r="F226" s="21">
         <v>31.5</v>
       </c>
       <c r="G226" s="6">
@@ -10927,7 +10927,7 @@
       <c r="E227" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F227" s="25">
+      <c r="F227" s="21">
         <v>31.05</v>
       </c>
       <c r="G227" s="6">
@@ -10959,7 +10959,7 @@
       <c r="E228" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F228" s="25">
+      <c r="F228" s="21">
         <v>30.04</v>
       </c>
       <c r="G228" s="6">
@@ -10991,7 +10991,7 @@
       <c r="E229" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F229" s="24">
+      <c r="F229" s="20">
         <v>393.75</v>
       </c>
       <c r="G229" s="15">
@@ -11023,7 +11023,7 @@
       <c r="E230" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F230" s="25">
+      <c r="F230" s="21">
         <v>30.04</v>
       </c>
       <c r="G230" s="6">
@@ -11055,7 +11055,7 @@
       <c r="E231" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F231" s="25">
+      <c r="F231" s="21">
         <v>30.04</v>
       </c>
       <c r="G231" s="6">
@@ -11087,7 +11087,7 @@
       <c r="E232" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F232" s="25">
+      <c r="F232" s="21">
         <v>30.04</v>
       </c>
       <c r="G232" s="6">
@@ -11119,7 +11119,7 @@
       <c r="E233" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F233" s="25">
+      <c r="F233" s="21">
         <v>30.04</v>
       </c>
       <c r="G233" s="6">
@@ -11151,330 +11151,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53D5A8D-0D87-45D9-9FF6-6E6D9F3C37EE}">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>201</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="25">
-        <v>1763370</v>
-      </c>
-      <c r="G2" s="6">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="6">
-        <v>927616</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2392</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="25">
-        <v>1114923.6000000001</v>
-      </c>
-      <c r="G3" s="6">
-        <v>5</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="6">
-        <v>927295</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>2708</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" s="25">
-        <v>98789.67</v>
-      </c>
-      <c r="G4" s="6">
-        <v>5</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="6">
-        <v>927346</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>5005</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="F5" s="25">
-        <v>97380.89</v>
-      </c>
-      <c r="G5" s="6">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="6">
-        <v>930280</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5005</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="25">
-        <v>47889.45</v>
-      </c>
-      <c r="G6" s="6">
-        <v>5</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="6">
-        <v>927398</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>3577</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="F7" s="25">
-        <v>12851.37</v>
-      </c>
-      <c r="G7" s="6">
-        <v>5</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="6">
-        <v>928309</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>4597</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="25">
-        <v>4725</v>
-      </c>
-      <c r="G8" s="6">
-        <v>5</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="6">
-        <v>927395</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>3612</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="25">
-        <v>1023.75</v>
-      </c>
-      <c r="G9" s="6">
-        <v>5</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="6">
-        <v>927347</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J257"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
@@ -11485,18 +11173,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>501</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -11818,7 +11506,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>2901</v>
       </c>
@@ -12106,7 +11794,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>3118</v>
       </c>
@@ -12426,7 +12114,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>3612</v>
       </c>
@@ -12778,7 +12466,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>1168</v>
       </c>
@@ -12842,7 +12530,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>2708</v>
       </c>
@@ -13034,7 +12722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>4677</v>
       </c>
@@ -13162,7 +12850,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>1718</v>
       </c>
@@ -13194,7 +12882,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>1718</v>
       </c>
@@ -13226,7 +12914,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>1718</v>
       </c>
@@ -13258,7 +12946,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>1718</v>
       </c>
@@ -13290,7 +12978,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>1718</v>
       </c>
@@ -13322,7 +13010,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>1718</v>
       </c>
@@ -13450,7 +13138,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>451</v>
       </c>
@@ -13834,7 +13522,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>2423</v>
       </c>
@@ -13866,7 +13554,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>2423</v>
       </c>
@@ -13898,7 +13586,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>2423</v>
       </c>
@@ -14090,7 +13778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>11560</v>
       </c>
@@ -14346,7 +14034,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>752</v>
       </c>
@@ -14826,7 +14514,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>3128</v>
       </c>
@@ -14858,7 +14546,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>3128</v>
       </c>
@@ -14890,7 +14578,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="9">
         <v>3128</v>
       </c>
@@ -16138,7 +15826,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="9">
         <v>2962</v>
       </c>
@@ -16586,7 +16274,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="9">
         <v>5005</v>
       </c>
@@ -17290,7 +16978,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="9">
         <v>208</v>
       </c>
@@ -17418,7 +17106,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="9">
         <v>13672</v>
       </c>
@@ -17610,7 +17298,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="9">
         <v>3239</v>
       </c>
@@ -18282,7 +17970,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="9">
         <v>5186</v>
       </c>
@@ -18442,7 +18130,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="9">
         <v>2690</v>
       </c>
@@ -18474,7 +18162,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="9">
         <v>2690</v>
       </c>
@@ -18506,7 +18194,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="9">
         <v>2690</v>
       </c>
@@ -18602,7 +18290,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="9">
         <v>4597</v>
       </c>
@@ -19082,7 +18770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="9">
         <v>2458</v>
       </c>
@@ -19338,7 +19026,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="9">
         <v>201</v>
       </c>
@@ -19659,6 +19347,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:J257" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Pago"/>
+        <filter val="Parcelado"/>
+        <filter val="Status 1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
@@ -19666,7 +19363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J71"/>
   <sheetViews>
@@ -19688,18 +19385,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>859</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -21917,7 +21614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I262"/>
   <sheetViews>
@@ -21938,17 +21635,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>860</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">

</xml_diff>